<commit_message>
Checked for multiple inputs and made changes in fetching patient name.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://avaalisolutions-my.sharepoint.com/personal/sameer_shariff_avaali_com/Documents/Documents/UiPath/LabTest/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD61B013-4DB3-481D-B995-47B72CEABB30}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A22EA19-ADF7-4C21-A6D1-606224C8CDAA}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -214,6 +214,18 @@
   </si>
   <si>
     <t>OutlookMailAccountToAccess</t>
+  </si>
+  <si>
+    <t>D:\uipath\Lab Test Reports Automation Shared Folder\Output</t>
+  </si>
+  <si>
+    <t>Master Datatable Excel Path</t>
+  </si>
+  <si>
+    <t>Master Datatable Excel sheet name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reports Status </t>
   </si>
 </sst>
 </file>
@@ -290,6 +302,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -592,7 +608,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -749,23 +765,37 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>

</xml_diff>